<commit_message>
Excel Download and Upload feature
</commit_message>
<xml_diff>
--- a/src/main/files/FinalSheet.xlsx
+++ b/src/main/files/FinalSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pani Vignesh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88B8549-BC12-400C-B988-1D3810ABF094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5DFB73-5B35-4173-9B4C-FF0F4532A41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{068F22AC-8C7B-4D5C-838D-2820B7C4FCF1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>SL.NO</t>
   </si>
@@ -63,34 +63,28 @@
     <t>Testing the app</t>
   </si>
   <si>
-    <t>Elango</t>
-  </si>
-  <si>
     <t>Test email for Java App</t>
   </si>
   <si>
-    <t>Hey Senior Dev Elango Hope you got this email..</t>
-  </si>
-  <si>
     <t>panivignesh@yahoo.in</t>
   </si>
   <si>
     <t>Pani</t>
   </si>
   <si>
+    <t>Hey Senior Dev Elango Hope you got this email.. With Attachment</t>
+  </si>
+  <si>
     <t>takrawelangogmail.com</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>name is valid |email id is valid |dateOfBirth id is valid |subject is valid |content is valid |</t>
-  </si>
-  <si>
     <t>Mail Sent</t>
   </si>
   <si>
-    <t>name is valid |email id is invalid |dateOfBirth id is valid |subject is valid |content is valid |</t>
+    <t xml:space="preserve"> Email ID is invalid | Name is empty |</t>
   </si>
 </sst>
 </file>
@@ -462,7 +456,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,13 +498,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4">
-        <v>34885</v>
+        <v>35602</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -519,30 +513,27 @@
         <v>8</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="4">
         <v>35597</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>